<commit_message>
feat:  final initial solution
</commit_message>
<xml_diff>
--- a/Results/d_1_2_3_comparison_init_no_init_no_init_time_limit.xlsx
+++ b/Results/d_1_2_3_comparison_init_no_init_no_init_time_limit.xlsx
@@ -5,17 +5,21 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcoturetta/Projects/trees/Results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcoturetta/Projects/trees_backup/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D647499B-125F-4944-9AE3-163B27C303A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8866C8A-CA34-7F47-99AB-049EB977550D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-2140" windowWidth="38400" windowHeight="19560" activeTab="2" xr2:uid="{6FABF61E-5EBE-E440-8258-C5C2D179FD09}"/>
+    <workbookView xWindow="29100" yWindow="-2140" windowWidth="38400" windowHeight="19560" activeTab="6" xr2:uid="{6FABF61E-5EBE-E440-8258-C5C2D179FD09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="d1" sheetId="4" r:id="rId4"/>
+    <sheet name="d2" sheetId="5" r:id="rId5"/>
+    <sheet name="d3" sheetId="6" r:id="rId6"/>
+    <sheet name="d4" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="res_continuous_2023_03_17" localSheetId="0">Sheet1!$A$2:$K$32</definedName>
@@ -23,6 +27,10 @@
     <definedName name="res_continuous_2023_03_21" localSheetId="1">Sheet2!$A$2:$L$16</definedName>
     <definedName name="res_continuous_2023_03_21_1" localSheetId="1">Sheet2!$A$18:$O$32</definedName>
     <definedName name="res_continuous_2023_03_21_1" localSheetId="2">Sheet3!$A$2:$L$16</definedName>
+    <definedName name="res_continuous_2023_03_22" localSheetId="3">'d1'!$A$2:$K$16</definedName>
+    <definedName name="res_continuous_2023_03_22" localSheetId="4">'d2'!$A$2:$K$16</definedName>
+    <definedName name="res_continuous_2023_03_22" localSheetId="5">'d3'!$A$2:$K$16</definedName>
+    <definedName name="res_continuous_2023_03_22" localSheetId="6">'d4'!$A$2:$K$16</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -91,7 +99,7 @@
     </textPr>
   </connection>
   <connection id="3" xr16:uid="{F61C3614-5D58-794E-A653-93BAA3E6D644}" name="res_continuous_2023-03-21" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/marcoturetta/Projects/trees/Results/res_continuous_2023-03-21.csv" comma="1">
+    <textPr sourceFile="/Users/marcoturetta/Projects/trees/Results/res_continuous_2023-03-21.csv" comma="1">
       <textFields count="15">
         <textField/>
         <textField/>
@@ -112,7 +120,7 @@
     </textPr>
   </connection>
   <connection id="4" xr16:uid="{12312042-73BB-D546-B368-D7584038647F}" name="res_continuous_2023-03-211" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/marcoturetta/Projects/trees/Results/res_continuous_2023-03-21.csv" comma="1">
+    <textPr sourceFile="/Users/marcoturetta/Projects/trees/Results/res_continuous_2023-03-21.csv" comma="1">
       <textFields count="15">
         <textField/>
         <textField/>
@@ -133,7 +141,91 @@
     </textPr>
   </connection>
   <connection id="5" xr16:uid="{72CBC193-DF90-DA48-AAAD-1827DB3CD0D2}" name="res_continuous_2023-03-2111" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/marcoturetta/Projects/trees/Results/res_continuous_2023-03-21.csv" comma="1">
+    <textPr sourceFile="/Users/marcoturetta/Projects/trees/Results/res_continuous_2023-03-21.csv" comma="1">
+      <textFields count="15">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" xr16:uid="{2219E069-800F-FB4C-999B-4D01E79E33A4}" name="res_continuous_2023-03-22" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/marcoturetta/Projects/trees_backup/Results/res_continuous_2023-03-22.csv" comma="1">
+      <textFields count="15">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" xr16:uid="{53E8F1B5-C132-A144-BDC5-F74B95195479}" name="res_continuous_2023-03-221" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/marcoturetta/Projects/trees_backup/Results/res_continuous_2023-03-22.csv" comma="1">
+      <textFields count="15">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="8" xr16:uid="{8E23A30B-453B-664B-9867-B92BACDFE696}" name="res_continuous_2023-03-222" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/marcoturetta/Projects/trees_backup/Results/res_continuous_2023-03-22.csv" comma="1">
+      <textFields count="15">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="9" xr16:uid="{0E911E47-3104-394A-B619-8A4604585186}" name="res_continuous_2023-03-223" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/marcoturetta/Projects/trees_backup/Results/res_continuous_2023-03-22.csv" comma="1">
       <textFields count="15">
         <textField/>
         <textField/>
@@ -157,7 +249,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="34">
   <si>
     <t>yacht_hydrodynamics_reg.csv</t>
   </si>
@@ -248,6 +340,18 @@
   <si>
     <t>[False]</t>
   </si>
+  <si>
+    <t>initial solution</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>initialization time</t>
+  </si>
 </sst>
 </file>
 
@@ -301,11 +405,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -324,23 +429,39 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="res_continuous_2023-03-17" connectionId="1" xr16:uid="{001C276C-1108-EC48-9063-24A6196E6C73}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="res_continuous_2023-03-18" connectionId="2" xr16:uid="{78CB4E18-9BB6-D34D-9177-678E75660766}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="res_continuous_2023-03-17" connectionId="1" xr16:uid="{001C276C-1108-EC48-9063-24A6196E6C73}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="res_continuous_2023_03_21_1" connectionId="4" xr16:uid="{BA017236-576A-1543-BD2D-FC4FFAFCBA2B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="res_continuous_2023-03-21" connectionId="3" xr16:uid="{DA90511F-46E1-864E-9F44-FE92330B9747}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="res_continuous_2023-03-21" connectionId="3" xr16:uid="{DA90511F-46E1-864E-9F44-FE92330B9747}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="res_continuous_2023_03_21_1" connectionId="4" xr16:uid="{BA017236-576A-1543-BD2D-FC4FFAFCBA2B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="res_continuous_2023_03_21_1" connectionId="5" xr16:uid="{B01E4D8D-B577-EE45-B822-75DA8EB11D48}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="res_continuous_2023-03-22" connectionId="6" xr16:uid="{A5D38850-8ACE-B74B-A1F6-1DB61CF3BEA5}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="res_continuous_2023-03-22" connectionId="7" xr16:uid="{5939C551-5B47-984D-8403-7AC38DECB97D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="res_continuous_2023-03-22" connectionId="8" xr16:uid="{750810FD-BE1B-3847-9B2A-75BDF00C35CF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="res_continuous_2023-03-22" connectionId="9" xr16:uid="{EABDB209-7D94-D04F-B7C9-522F40F33E86}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3627,8 +3748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2F320B-2CF1-614B-B643-7448000E355E}">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4251,4 +4372,2363 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25CABA91-DA58-7347-B01E-66DDF933C3C2}">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="6.5" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" customWidth="1"/>
+    <col min="10" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>4176</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>71.585846900939899</v>
+      </c>
+      <c r="F2">
+        <v>5.8064157251868198E-2</v>
+      </c>
+      <c r="G2">
+        <v>0.51896274526930997</v>
+      </c>
+      <c r="H2">
+        <v>5.6567033257232897E-2</v>
+      </c>
+      <c r="I2">
+        <v>0.53593631514551099</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2">
+        <v>59.925750017166102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4176</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>360</v>
+      </c>
+      <c r="E3">
+        <v>413.30565595626803</v>
+      </c>
+      <c r="F3">
+        <v>5.4591450634970597E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.51443699730631098</v>
+      </c>
+      <c r="H3">
+        <v>5.2376340130824997E-2</v>
+      </c>
+      <c r="I3">
+        <v>0.546584896413846</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3">
+        <v>46.067264795303302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4176</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>360</v>
+      </c>
+      <c r="E4">
+        <v>364.96678209304798</v>
+      </c>
+      <c r="F4">
+        <v>5.5619410361688597E-2</v>
+      </c>
+      <c r="G4">
+        <v>0.53036671249618705</v>
+      </c>
+      <c r="H4">
+        <v>5.3566090037466103E-2</v>
+      </c>
+      <c r="I4">
+        <v>0.55801243305320003</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1502</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>15.259091377258301</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.101037318487485</v>
+      </c>
+      <c r="G5">
+        <v>0.524154724101623</v>
+      </c>
+      <c r="H5">
+        <v>9.3757599872394501E-2</v>
+      </c>
+      <c r="I5">
+        <v>0.50524105805886399</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5">
+        <v>12.657376050949001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1502</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>360</v>
+      </c>
+      <c r="E6">
+        <v>374.51696491241398</v>
+      </c>
+      <c r="F6">
+        <v>8.3734515733796894E-2</v>
+      </c>
+      <c r="G6">
+        <v>0.633342659907004</v>
+      </c>
+      <c r="H6">
+        <v>8.2814292993655295E-2</v>
+      </c>
+      <c r="I6">
+        <v>0.57889698400530198</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6">
+        <v>12.2244679927825</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1502</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>360</v>
+      </c>
+      <c r="E7">
+        <v>361.351740837097</v>
+      </c>
+      <c r="F7">
+        <v>8.3379827812867E-2</v>
+      </c>
+      <c r="G7">
+        <v>0.64513606718590299</v>
+      </c>
+      <c r="H7">
+        <v>8.1154430823851806E-2</v>
+      </c>
+      <c r="I7">
+        <v>0.59834568285551604</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>391</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>10.174567222595201</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.193341362757184</v>
+      </c>
+      <c r="G8">
+        <v>0.49043728085876298</v>
+      </c>
+      <c r="H8">
+        <v>0.214109427814864</v>
+      </c>
+      <c r="I8">
+        <v>0.41001560310406898</v>
+      </c>
+      <c r="J8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8">
+        <v>9.3851857185363698</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>391</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>360</v>
+      </c>
+      <c r="E9">
+        <v>373.90707087516699</v>
+      </c>
+      <c r="F9">
+        <v>0.18624054045555899</v>
+      </c>
+      <c r="G9">
+        <v>0.35081479440545399</v>
+      </c>
+      <c r="H9">
+        <v>0.23477554028109399</v>
+      </c>
+      <c r="I9">
+        <v>0.219063605839079</v>
+      </c>
+      <c r="J9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9">
+        <v>12.6975889205932</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>391</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>360</v>
+      </c>
+      <c r="E10">
+        <v>360.48158884048399</v>
+      </c>
+      <c r="F10">
+        <v>0.150924856466183</v>
+      </c>
+      <c r="G10">
+        <v>0.473597746626511</v>
+      </c>
+      <c r="H10">
+        <v>0.192053877228791</v>
+      </c>
+      <c r="I10">
+        <v>0.33352289216839298</v>
+      </c>
+      <c r="J10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>4897</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>107.744113922119</v>
+      </c>
+      <c r="F11">
+        <v>9.6587734170940201E-2</v>
+      </c>
+      <c r="G11">
+        <v>0.30158466572772902</v>
+      </c>
+      <c r="H11">
+        <v>9.8168695814899606E-2</v>
+      </c>
+      <c r="I11">
+        <v>0.30701362207143901</v>
+      </c>
+      <c r="J11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11">
+        <v>96.433967828750596</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>4897</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>360</v>
+      </c>
+      <c r="E12">
+        <v>446.61713981628401</v>
+      </c>
+      <c r="F12">
+        <v>9.6358448658171197E-2</v>
+      </c>
+      <c r="G12">
+        <v>0.28049753708394798</v>
+      </c>
+      <c r="H12">
+        <v>9.66809390961932E-2</v>
+      </c>
+      <c r="I12">
+        <v>0.29483234582729101</v>
+      </c>
+      <c r="J12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12">
+        <v>73.702027082443195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>4897</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>360</v>
+      </c>
+      <c r="E13">
+        <v>367.421705245971</v>
+      </c>
+      <c r="F13">
+        <v>9.6358448658171197E-2</v>
+      </c>
+      <c r="G13">
+        <v>0.28049753708394798</v>
+      </c>
+      <c r="H13">
+        <v>9.66809390961932E-2</v>
+      </c>
+      <c r="I13">
+        <v>0.29483234582729101</v>
+      </c>
+      <c r="J13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>307</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>7.7512829303741402</v>
+      </c>
+      <c r="F14" s="4">
+        <v>4.7020424408479401E-2</v>
+      </c>
+      <c r="G14">
+        <v>0.88130791676074005</v>
+      </c>
+      <c r="H14">
+        <v>4.3295118766224203E-2</v>
+      </c>
+      <c r="I14">
+        <v>0.90945530809714104</v>
+      </c>
+      <c r="J14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14">
+        <v>7.2819240093231201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>307</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>360</v>
+      </c>
+      <c r="E15">
+        <v>367.977332115173</v>
+      </c>
+      <c r="F15">
+        <v>2.0894071063046901E-2</v>
+      </c>
+      <c r="G15">
+        <v>0.97908382671898597</v>
+      </c>
+      <c r="H15">
+        <v>2.2867234527443301E-2</v>
+      </c>
+      <c r="I15">
+        <v>0.975887492056837</v>
+      </c>
+      <c r="J15" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15">
+        <v>7.2683680057525599</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>307</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>360</v>
+      </c>
+      <c r="E16">
+        <v>360.41126704215998</v>
+      </c>
+      <c r="F16">
+        <v>2.0525929695595399E-2</v>
+      </c>
+      <c r="G16">
+        <v>0.97984374941335195</v>
+      </c>
+      <c r="H16">
+        <v>2.0748809110987101E-2</v>
+      </c>
+      <c r="I16">
+        <v>0.98611904649404702</v>
+      </c>
+      <c r="J16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K16">
+    <sortCondition ref="A2:A16"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A27BE53-1FF4-3248-9EDF-CE912A7FFCD7}">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="5.5" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.5" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" customWidth="1"/>
+    <col min="9" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>4176</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>118.990724802017</v>
+      </c>
+      <c r="F2">
+        <v>5.7862971573451598E-2</v>
+      </c>
+      <c r="G2">
+        <v>0.52104963159800799</v>
+      </c>
+      <c r="H2">
+        <v>5.6912091880954203E-2</v>
+      </c>
+      <c r="I2">
+        <v>0.52697094905314601</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2">
+        <v>98.188777208328204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4176</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>360</v>
+      </c>
+      <c r="E3">
+        <v>442.50428128242402</v>
+      </c>
+      <c r="F3">
+        <v>5.7862971573451598E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.52104963159800799</v>
+      </c>
+      <c r="H3">
+        <v>5.6912091880954203E-2</v>
+      </c>
+      <c r="I3">
+        <v>0.52697094905314601</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3">
+        <v>65.429152965545597</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4176</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>360</v>
+      </c>
+      <c r="E4">
+        <v>373.561773777008</v>
+      </c>
+      <c r="F4">
+        <v>0.32094739093242097</v>
+      </c>
+      <c r="G4">
+        <v>-7.6440400366359302</v>
+      </c>
+      <c r="H4">
+        <v>0.31130382775119603</v>
+      </c>
+      <c r="I4">
+        <v>-7.89051796655479</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1502</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>28.9274578094482</v>
+      </c>
+      <c r="F5">
+        <v>0.10154237523802</v>
+      </c>
+      <c r="G5">
+        <v>0.53920518235564296</v>
+      </c>
+      <c r="H5">
+        <v>9.4220216332376094E-2</v>
+      </c>
+      <c r="I5">
+        <v>0.52054801746455903</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5">
+        <v>21.424167871475198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1502</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>360</v>
+      </c>
+      <c r="E6">
+        <v>389.32599902152998</v>
+      </c>
+      <c r="F6">
+        <v>9.3913281499613005E-2</v>
+      </c>
+      <c r="G6">
+        <v>0.52569794811142001</v>
+      </c>
+      <c r="H6">
+        <v>9.1802521671797394E-2</v>
+      </c>
+      <c r="I6">
+        <v>0.49123367045689997</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6">
+        <v>21.214681863784701</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1502</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>360</v>
+      </c>
+      <c r="E7">
+        <v>364.01280879974303</v>
+      </c>
+      <c r="F7">
+        <v>2.3171280439529802</v>
+      </c>
+      <c r="G7">
+        <v>-61193.275906120303</v>
+      </c>
+      <c r="H7">
+        <v>4.8911262612985604</v>
+      </c>
+      <c r="I7">
+        <v>-111591.659900375</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>391</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>17.632429122924801</v>
+      </c>
+      <c r="F8">
+        <v>0.177495438391959</v>
+      </c>
+      <c r="G8">
+        <v>0.52004877099864799</v>
+      </c>
+      <c r="H8">
+        <v>0.206051207507218</v>
+      </c>
+      <c r="I8">
+        <v>0.42619201111861399</v>
+      </c>
+      <c r="J8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8">
+        <v>15.3877041339874</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>391</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>360</v>
+      </c>
+      <c r="E9">
+        <v>382.66651105880698</v>
+      </c>
+      <c r="F9">
+        <v>0.13865720318981301</v>
+      </c>
+      <c r="G9">
+        <v>0.49440063952207702</v>
+      </c>
+      <c r="H9">
+        <v>0.17251691947454401</v>
+      </c>
+      <c r="I9">
+        <v>0.39645442566530897</v>
+      </c>
+      <c r="J9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9">
+        <v>20.603351116180399</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>391</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>360</v>
+      </c>
+      <c r="E10">
+        <v>361.369428157806</v>
+      </c>
+      <c r="F10">
+        <v>0.19319551883868399</v>
+      </c>
+      <c r="G10">
+        <v>0.53088592213244301</v>
+      </c>
+      <c r="H10">
+        <v>0.56305730918509</v>
+      </c>
+      <c r="I10">
+        <v>-29.567245488699299</v>
+      </c>
+      <c r="J10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>4897</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>177.98407602310101</v>
+      </c>
+      <c r="F11">
+        <v>9.5690657323454803E-2</v>
+      </c>
+      <c r="G11">
+        <v>0.31388955649650402</v>
+      </c>
+      <c r="H11">
+        <v>9.7650056065033297E-2</v>
+      </c>
+      <c r="I11">
+        <v>0.31193032407043503</v>
+      </c>
+      <c r="J11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11">
+        <v>151.776081323623</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>4897</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>360</v>
+      </c>
+      <c r="E12">
+        <v>546.26957798004105</v>
+      </c>
+      <c r="F12">
+        <v>9.5690657323454803E-2</v>
+      </c>
+      <c r="G12">
+        <v>0.31388955649650402</v>
+      </c>
+      <c r="H12">
+        <v>9.7650056065033297E-2</v>
+      </c>
+      <c r="I12">
+        <v>0.31193032407043503</v>
+      </c>
+      <c r="J12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12">
+        <v>147.580837011337</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>4897</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>360</v>
+      </c>
+      <c r="E13">
+        <v>375.21211981773303</v>
+      </c>
+      <c r="F13">
+        <v>0.48170368479278303</v>
+      </c>
+      <c r="G13">
+        <v>-10.6761460661911</v>
+      </c>
+      <c r="H13">
+        <v>0.47142857142856998</v>
+      </c>
+      <c r="I13">
+        <v>-10.140713916192601</v>
+      </c>
+      <c r="J13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>307</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>9.7438499927520699</v>
+      </c>
+      <c r="F14">
+        <v>5.8850542847911601E-2</v>
+      </c>
+      <c r="G14">
+        <v>0.81003366792484799</v>
+      </c>
+      <c r="H14">
+        <v>5.6843502449295799E-2</v>
+      </c>
+      <c r="I14">
+        <v>0.83975224008588101</v>
+      </c>
+      <c r="J14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14">
+        <v>8.7157728672027499</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>307</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>360</v>
+      </c>
+      <c r="E15">
+        <v>372.46783709525999</v>
+      </c>
+      <c r="F15">
+        <v>1.9604272421354402E-2</v>
+      </c>
+      <c r="G15">
+        <v>0.98035007862464896</v>
+      </c>
+      <c r="H15">
+        <v>2.7535858971246899E-2</v>
+      </c>
+      <c r="I15">
+        <v>0.96930708584916503</v>
+      </c>
+      <c r="J15" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15">
+        <v>10.9759149551391</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>307</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>360</v>
+      </c>
+      <c r="E16">
+        <v>361.05124402046198</v>
+      </c>
+      <c r="F16">
+        <v>1.6004104251722599E-2</v>
+      </c>
+      <c r="G16">
+        <v>0.98540249200900598</v>
+      </c>
+      <c r="H16">
+        <v>2.2786844252660299E-2</v>
+      </c>
+      <c r="I16">
+        <v>0.97837027175400104</v>
+      </c>
+      <c r="J16" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K16">
+    <sortCondition ref="A2:A16"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4611DCE-A0B4-2C47-B9B9-6C543C1CEED3}">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="5.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" customWidth="1"/>
+    <col min="8" max="8" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>4176</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>161.749239921569</v>
+      </c>
+      <c r="F2">
+        <v>5.9037163940816297E-2</v>
+      </c>
+      <c r="G2">
+        <v>0.50321233075070804</v>
+      </c>
+      <c r="H2">
+        <v>5.8254085159011801E-2</v>
+      </c>
+      <c r="I2">
+        <v>0.50663592716328398</v>
+      </c>
+      <c r="J2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2">
+        <v>117.530268907547</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4176</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>360</v>
+      </c>
+      <c r="E3">
+        <v>494.62484502792302</v>
+      </c>
+      <c r="F3">
+        <v>5.9037163940816297E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.50321233075070804</v>
+      </c>
+      <c r="H3">
+        <v>5.8254085159011801E-2</v>
+      </c>
+      <c r="I3">
+        <v>0.50663592716328398</v>
+      </c>
+      <c r="J3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3">
+        <v>91.393648862838702</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4176</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>360</v>
+      </c>
+      <c r="E4">
+        <v>385.56003022193897</v>
+      </c>
+      <c r="F4">
+        <v>1.0559875494778901</v>
+      </c>
+      <c r="G4">
+        <v>-247856.79278030799</v>
+      </c>
+      <c r="H4">
+        <v>12.032755049888999</v>
+      </c>
+      <c r="I4">
+        <v>-3255543.1227432098</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1502</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>49.496955871582003</v>
+      </c>
+      <c r="F5">
+        <v>9.5892858461266994E-2</v>
+      </c>
+      <c r="G5">
+        <v>0.58101301516835002</v>
+      </c>
+      <c r="H5">
+        <v>8.9921351139456498E-2</v>
+      </c>
+      <c r="I5">
+        <v>0.55803051643693102</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5">
+        <v>34.445520877838099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1502</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>360</v>
+      </c>
+      <c r="E6">
+        <v>393.75802278518597</v>
+      </c>
+      <c r="F6">
+        <v>8.5101290363385804E-2</v>
+      </c>
+      <c r="G6">
+        <v>0.57557657298693599</v>
+      </c>
+      <c r="H6">
+        <v>8.7729968627484403E-2</v>
+      </c>
+      <c r="I6">
+        <v>0.51609351569580497</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6">
+        <v>21.406341791152901</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1502</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>360</v>
+      </c>
+      <c r="E7">
+        <v>367.04003787040699</v>
+      </c>
+      <c r="F7">
+        <v>152.98974290968201</v>
+      </c>
+      <c r="G7">
+        <v>-4069572.14004476</v>
+      </c>
+      <c r="H7">
+        <v>119.977518564272</v>
+      </c>
+      <c r="I7">
+        <v>-3512974.7778805601</v>
+      </c>
+      <c r="J7" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>391</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>44.7974948883056</v>
+      </c>
+      <c r="F8">
+        <v>0.16909373344226999</v>
+      </c>
+      <c r="G8">
+        <v>0.54633607973268705</v>
+      </c>
+      <c r="H8">
+        <v>0.19937999182846</v>
+      </c>
+      <c r="I8">
+        <v>0.43636342866390498</v>
+      </c>
+      <c r="J8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8">
+        <v>40.589566946029599</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>391</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>360</v>
+      </c>
+      <c r="E9">
+        <v>380.59534287452698</v>
+      </c>
+      <c r="F9">
+        <v>0.152428476268087</v>
+      </c>
+      <c r="G9">
+        <v>0.43418812083906999</v>
+      </c>
+      <c r="H9">
+        <v>0.20495817070463501</v>
+      </c>
+      <c r="I9">
+        <v>0.16299714284108699</v>
+      </c>
+      <c r="J9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9">
+        <v>17.110434770584099</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>391</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>360</v>
+      </c>
+      <c r="E10">
+        <v>362.50643706321699</v>
+      </c>
+      <c r="F10">
+        <v>3.9441304881350101</v>
+      </c>
+      <c r="G10">
+        <v>-5186.1325942234898</v>
+      </c>
+      <c r="H10">
+        <v>2.1729527214789002</v>
+      </c>
+      <c r="I10">
+        <v>-1723.11884227825</v>
+      </c>
+      <c r="J10" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>4897</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>284.33032989501902</v>
+      </c>
+      <c r="F11">
+        <v>9.40078574035174E-2</v>
+      </c>
+      <c r="G11">
+        <v>0.33141792517538898</v>
+      </c>
+      <c r="H11">
+        <v>9.6918915395163605E-2</v>
+      </c>
+      <c r="I11">
+        <v>0.31687312997271899</v>
+      </c>
+      <c r="J11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11">
+        <v>221.79754114151001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>4897</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>360</v>
+      </c>
+      <c r="E12">
+        <v>636.45779991149902</v>
+      </c>
+      <c r="F12">
+        <v>9.40078574035174E-2</v>
+      </c>
+      <c r="G12">
+        <v>0.33141792517538898</v>
+      </c>
+      <c r="H12">
+        <v>9.6918915395163605E-2</v>
+      </c>
+      <c r="I12">
+        <v>0.31687312997271899</v>
+      </c>
+      <c r="J12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12">
+        <v>214.13684582710201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>4897</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>360</v>
+      </c>
+      <c r="E13">
+        <v>388.17454409599299</v>
+      </c>
+      <c r="F13">
+        <v>0.48170368479278303</v>
+      </c>
+      <c r="G13">
+        <v>-10.6761460661911</v>
+      </c>
+      <c r="H13">
+        <v>0.47142857142856998</v>
+      </c>
+      <c r="I13">
+        <v>-10.140713916192601</v>
+      </c>
+      <c r="J13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>307</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>22.1592488288879</v>
+      </c>
+      <c r="F14">
+        <v>6.7121600695407804E-2</v>
+      </c>
+      <c r="G14">
+        <v>0.75615012664320602</v>
+      </c>
+      <c r="H14">
+        <v>7.2324356339505805E-2</v>
+      </c>
+      <c r="I14">
+        <v>0.74115712290518299</v>
+      </c>
+      <c r="J14" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14">
+        <v>14.894655942916801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>307</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>360</v>
+      </c>
+      <c r="E15">
+        <v>382.04294395446698</v>
+      </c>
+      <c r="F15">
+        <v>2.0732028680785601E-2</v>
+      </c>
+      <c r="G15">
+        <v>0.96460600602508395</v>
+      </c>
+      <c r="H15">
+        <v>2.1185517540488301</v>
+      </c>
+      <c r="I15">
+        <v>-1161.2125456685001</v>
+      </c>
+      <c r="J15" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15">
+        <v>18.858574151992698</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>307</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>360</v>
+      </c>
+      <c r="E16">
+        <v>362.93051528930602</v>
+      </c>
+      <c r="F16">
+        <v>12.085418189917901</v>
+      </c>
+      <c r="G16">
+        <v>-34240.5054998005</v>
+      </c>
+      <c r="H16">
+        <v>14.1462094105425</v>
+      </c>
+      <c r="I16">
+        <v>-41634.2715660217</v>
+      </c>
+      <c r="J16" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K16">
+    <sortCondition ref="A2:A16"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42C3935D-E67F-364D-9940-2CF043121203}">
+  <dimension ref="A1:K16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="8" max="8" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>4176</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>298.185586929321</v>
+      </c>
+      <c r="F2">
+        <v>5.5677894035133402E-2</v>
+      </c>
+      <c r="G2">
+        <v>0.53682563121721905</v>
+      </c>
+      <c r="H2">
+        <v>5.5396652010914801E-2</v>
+      </c>
+      <c r="I2">
+        <v>0.53164886071238504</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2">
+        <v>198.528312206268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>4176</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>360</v>
+      </c>
+      <c r="E3">
+        <v>623.36918926239002</v>
+      </c>
+      <c r="F3">
+        <v>5.5677894035133402E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.53682563121721905</v>
+      </c>
+      <c r="H3">
+        <v>5.5396652010914801E-2</v>
+      </c>
+      <c r="I3">
+        <v>0.53164886071238504</v>
+      </c>
+      <c r="J3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <v>173.36924219131399</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4176</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>360</v>
+      </c>
+      <c r="E4">
+        <v>413.39738512039099</v>
+      </c>
+      <c r="F4">
+        <v>1.05598780369291</v>
+      </c>
+      <c r="G4">
+        <v>-247820.62168305699</v>
+      </c>
+      <c r="H4">
+        <v>5.4321158366568201E-2</v>
+      </c>
+      <c r="I4">
+        <v>0.53452641124844003</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>1502</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>69.750046968459998</v>
+      </c>
+      <c r="F5">
+        <v>9.1053706873821305E-2</v>
+      </c>
+      <c r="G5">
+        <v>0.61968044936337296</v>
+      </c>
+      <c r="H5">
+        <v>8.7356816022082603E-2</v>
+      </c>
+      <c r="I5">
+        <v>0.58070735044671196</v>
+      </c>
+      <c r="J5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5">
+        <v>43.369040250778198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1502</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>360</v>
+      </c>
+      <c r="E6">
+        <v>413.46590399742098</v>
+      </c>
+      <c r="F6">
+        <v>8.73063799317393E-2</v>
+      </c>
+      <c r="G6">
+        <v>0.637671815910406</v>
+      </c>
+      <c r="H6">
+        <v>8.6152154462444702E-2</v>
+      </c>
+      <c r="I6">
+        <v>0.58379497927373902</v>
+      </c>
+      <c r="J6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6">
+        <v>29.340301752090401</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1502</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>360</v>
+      </c>
+      <c r="E7">
+        <v>376.65775394439697</v>
+      </c>
+      <c r="F7">
+        <v>10.087672523037099</v>
+      </c>
+      <c r="G7">
+        <v>-346222.14293109498</v>
+      </c>
+      <c r="H7">
+        <v>9.2450516017781301E-2</v>
+      </c>
+      <c r="I7">
+        <v>0.47141432857826099</v>
+      </c>
+      <c r="J7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>391</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>58.591569900512603</v>
+      </c>
+      <c r="F8">
+        <v>0.152371433009445</v>
+      </c>
+      <c r="G8">
+        <v>0.59294346851203805</v>
+      </c>
+      <c r="H8">
+        <v>0.187210023967568</v>
+      </c>
+      <c r="I8">
+        <v>0.47470613774056097</v>
+      </c>
+      <c r="J8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8">
+        <v>42.255343914031897</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>391</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>360</v>
+      </c>
+      <c r="E9">
+        <v>391.22403907775799</v>
+      </c>
+      <c r="F9">
+        <v>0.67109371649793703</v>
+      </c>
+      <c r="G9">
+        <v>-212.52801294180699</v>
+      </c>
+      <c r="H9">
+        <v>2.1392405063291098</v>
+      </c>
+      <c r="I9">
+        <v>-1846.8458233890201</v>
+      </c>
+      <c r="J9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9">
+        <v>23.377386093139599</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>391</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>360</v>
+      </c>
+      <c r="E10">
+        <v>366.04922413825898</v>
+      </c>
+      <c r="F10">
+        <v>4.7363741485948996</v>
+      </c>
+      <c r="G10">
+        <v>-4596.6696616193003</v>
+      </c>
+      <c r="H10">
+        <v>16.1760662109842</v>
+      </c>
+      <c r="I10">
+        <v>-25745.638475164898</v>
+      </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>4897</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>469.74882316589299</v>
+      </c>
+      <c r="F11">
+        <v>9.2556758372483602E-2</v>
+      </c>
+      <c r="G11">
+        <v>0.34986978501082899</v>
+      </c>
+      <c r="H11">
+        <v>9.6353055252005604E-2</v>
+      </c>
+      <c r="I11">
+        <v>0.31642269260918898</v>
+      </c>
+      <c r="J11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11">
+        <v>325.73391389846802</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>4897</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>360</v>
+      </c>
+      <c r="E12">
+        <v>766.89380502700806</v>
+      </c>
+      <c r="F12">
+        <v>9.2556758372483602E-2</v>
+      </c>
+      <c r="G12">
+        <v>0.34986978501082899</v>
+      </c>
+      <c r="H12">
+        <v>9.6353055252005604E-2</v>
+      </c>
+      <c r="I12">
+        <v>0.31642269260918898</v>
+      </c>
+      <c r="J12" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12">
+        <v>285.91834592819202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>4897</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>360</v>
+      </c>
+      <c r="E13">
+        <v>419.24000310897799</v>
+      </c>
+      <c r="F13">
+        <v>0.48170368479278303</v>
+      </c>
+      <c r="G13">
+        <v>-10.6761460661911</v>
+      </c>
+      <c r="H13">
+        <v>0.47142857142856998</v>
+      </c>
+      <c r="I13">
+        <v>-10.140713916192601</v>
+      </c>
+      <c r="J13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>307</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>38.114728927612298</v>
+      </c>
+      <c r="F14">
+        <v>6.7328914211905705E-2</v>
+      </c>
+      <c r="G14">
+        <v>0.75776786809946906</v>
+      </c>
+      <c r="H14">
+        <v>6.7560557329282706E-2</v>
+      </c>
+      <c r="I14">
+        <v>0.77578100077152201</v>
+      </c>
+      <c r="J14" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14">
+        <v>27.027063131332302</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>307</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>360</v>
+      </c>
+      <c r="E15">
+        <v>393.78319501876803</v>
+      </c>
+      <c r="F15">
+        <v>3.34984575397272</v>
+      </c>
+      <c r="G15">
+        <v>-10506.307618941801</v>
+      </c>
+      <c r="H15">
+        <v>13.671378999638399</v>
+      </c>
+      <c r="I15">
+        <v>-21471.253834627201</v>
+      </c>
+      <c r="J15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15">
+        <v>27.4768531322479</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>307</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>360</v>
+      </c>
+      <c r="E16">
+        <v>363.63542389869599</v>
+      </c>
+      <c r="F16">
+        <v>113.551163592059</v>
+      </c>
+      <c r="G16">
+        <v>-309234.10023765097</v>
+      </c>
+      <c r="H16">
+        <v>119.534251473059</v>
+      </c>
+      <c r="I16">
+        <v>-354583.64809843502</v>
+      </c>
+      <c r="J16" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K16">
+    <sortCondition ref="A2:A16"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>